<commit_message>
modified excel data of test cases
</commit_message>
<xml_diff>
--- a/Swab labs test cases.xlsx
+++ b/Swab labs test cases.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shimp\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shimp\OneDrive\Desktop\excel-data-swab labs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F215C3A3-A3C8-4C41-8CA9-7F44D6185016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D490AB2E-D237-4B19-8C0B-CA906CF208A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{F2389022-1145-44B2-9DA1-94ADD3AAD9EA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F2389022-1145-44B2-9DA1-94ADD3AAD9EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sceanario" sheetId="1" r:id="rId1"/>
-    <sheet name="Checkout" sheetId="6" r:id="rId2"/>
-    <sheet name="Your cart" sheetId="5" r:id="rId3"/>
+    <sheet name="Your cart" sheetId="5" r:id="rId2"/>
+    <sheet name="Checkout" sheetId="6" r:id="rId3"/>
     <sheet name="Filter" sheetId="4" r:id="rId4"/>
     <sheet name="Product" sheetId="2" r:id="rId5"/>
     <sheet name="Add to cart" sheetId="3" r:id="rId6"/>
@@ -665,7 +665,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1104,6 +1104,656 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B88AC9-0810-44A5-9807-E32954A756E4}">
+  <dimension ref="A1:K23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.77734375" customWidth="1"/>
+    <col min="2" max="2" width="22.21875" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.21875" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" customWidth="1"/>
+    <col min="9" max="9" width="17.21875" customWidth="1"/>
+    <col min="10" max="10" width="16.88671875" customWidth="1"/>
+    <col min="11" max="11" width="12.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+    </row>
+    <row r="3" spans="1:11" s="8" customFormat="1" ht="36" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+    </row>
+    <row r="4" spans="1:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+    </row>
+    <row r="5" spans="1:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+    </row>
+    <row r="6" spans="1:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+    </row>
+    <row r="7" spans="1:11" ht="90" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+    </row>
+    <row r="8" spans="1:11" ht="90" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+    </row>
+    <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+    </row>
+    <row r="10" spans="1:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+    </row>
+    <row r="11" spans="1:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+    </row>
+    <row r="12" spans="1:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+    </row>
+    <row r="13" spans="1:11" ht="90" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+    </row>
+    <row r="14" spans="1:11" ht="90" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+    </row>
+    <row r="15" spans="1:11" ht="90" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+    </row>
+    <row r="16" spans="1:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+    </row>
+    <row r="17" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+    </row>
+    <row r="18" spans="1:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+    </row>
+    <row r="19" spans="1:11" ht="90" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+    </row>
+    <row r="20" spans="1:11" ht="90" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+    </row>
+    <row r="21" spans="1:11" ht="90" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+    </row>
+    <row r="22" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A22" s="13"/>
+    </row>
+    <row r="23" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A23" s="13"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D314AB-E5D7-4813-95F3-7DF195B21AD5}">
   <dimension ref="A1:K5"/>
   <sheetViews>
@@ -1259,656 +1909,6 @@
       <c r="K5" s="11"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B88AC9-0810-44A5-9807-E32954A756E4}">
-  <dimension ref="A1:K23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.77734375" customWidth="1"/>
-    <col min="2" max="2" width="22.21875" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" customWidth="1"/>
-    <col min="6" max="6" width="26.21875" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" customWidth="1"/>
-    <col min="9" max="9" width="17.21875" customWidth="1"/>
-    <col min="10" max="10" width="16.88671875" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="36" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-    </row>
-    <row r="3" spans="1:11" s="8" customFormat="1" ht="36" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-    </row>
-    <row r="4" spans="1:11" ht="54" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-    </row>
-    <row r="5" spans="1:11" ht="54" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-    </row>
-    <row r="6" spans="1:11" ht="54" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-    </row>
-    <row r="7" spans="1:11" ht="90" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-    </row>
-    <row r="8" spans="1:11" ht="90" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-    </row>
-    <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-    </row>
-    <row r="10" spans="1:11" ht="54" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-    </row>
-    <row r="11" spans="1:11" ht="54" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-    </row>
-    <row r="12" spans="1:11" ht="54" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-    </row>
-    <row r="13" spans="1:11" ht="90" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-    </row>
-    <row r="14" spans="1:11" ht="90" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-    </row>
-    <row r="15" spans="1:11" ht="90" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-    </row>
-    <row r="16" spans="1:11" ht="54" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-    </row>
-    <row r="17" spans="1:11" ht="36" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-    </row>
-    <row r="18" spans="1:11" ht="54" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-    </row>
-    <row r="19" spans="1:11" ht="90" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-    </row>
-    <row r="20" spans="1:11" ht="90" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-    </row>
-    <row r="21" spans="1:11" ht="90" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-    </row>
-    <row r="22" spans="1:11" ht="18" x14ac:dyDescent="0.3">
-      <c r="A22" s="13"/>
-    </row>
-    <row r="23" spans="1:11" ht="18" x14ac:dyDescent="0.3">
-      <c r="A23" s="13"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2263,7 +2263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4D253F-B190-4545-926F-D8122D5A48E6}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>

</xml_diff>